<commit_message>
Update command list to 2.0 for 2.1.11 new dut version, after tested by Jerry
</commit_message>
<xml_diff>
--- a/R1_test_command_list_V2.0_for_2.1.11.xlsx
+++ b/R1_test_command_list_V2.0_for_2.1.11.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="278">
   <si>
     <t>./inventory.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1007,10 +1007,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>set_standby_mode.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/set_standby_mode.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1192,12 +1188,33 @@
     <t>push_file.bat &lt;file_name&gt; &lt;destination&gt; &lt;destination_path&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Added in 2.1.11, for reboot the system.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Added In 2.1.11 and newer version.  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell mount -o remount rw /</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D:\Fancy.Liu\Tool\Android&gt;adb shell mount -o remount rw /
+mount: /: cannot remount rw read-write, is write-protected.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set_standby_mode.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1288,8 +1305,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1330,6 +1355,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1414,10 +1444,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1512,6 +1545,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1527,20 +1572,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1843,10 +1880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1941,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>44</v>
@@ -1963,7 +2000,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>45</v>
@@ -2007,7 +2044,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>11</v>
@@ -2065,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
@@ -2087,7 +2124,7 @@
         <v>81</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>10</v>
@@ -2151,7 +2188,7 @@
         <v>146</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E14" s="17" t="s">
         <v>113</v>
@@ -2230,18 +2267,18 @@
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>236</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>237</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="17"/>
-      <c r="H18" s="11" t="s">
-        <v>271</v>
+      <c r="H18" s="10" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -2250,189 +2287,189 @@
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>238</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>239</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="11" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H19" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="35"/>
       <c r="B20" s="24">
         <v>18</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>86</v>
+      <c r="C20" s="17" t="s">
+        <v>262</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>220</v>
+        <v>263</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="17"/>
+        <v>40</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>228</v>
+      </c>
       <c r="G20" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+        <v>234</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="35"/>
       <c r="B21" s="24">
         <v>19</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>87</v>
+      <c r="C21" s="17" t="s">
+        <v>251</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>125</v>
+        <v>264</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="H21" s="27"/>
-    </row>
-    <row r="22" spans="1:8" ht="148.5" x14ac:dyDescent="0.15">
+        <v>252</v>
+      </c>
+      <c r="F21" s="21"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="35"/>
       <c r="B22" s="24">
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>149</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>159</v>
+        <v>84</v>
       </c>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="35"/>
       <c r="B23" s="24">
         <v>21</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>153</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>158</v>
+        <v>85</v>
       </c>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" ht="148.5" x14ac:dyDescent="0.15">
       <c r="A24" s="35"/>
       <c r="B24" s="24">
         <v>22</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>89</v>
+        <v>126</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>153</v>
+        <v>225</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>149</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="35"/>
       <c r="B25" s="24">
         <v>23</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>90</v>
+        <v>156</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>150</v>
+        <v>63</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>153</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H25" s="11"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>158</v>
+      </c>
+      <c r="H25" s="27"/>
+    </row>
+    <row r="26" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A26" s="35"/>
       <c r="B26" s="24">
         <v>24</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+        <v>157</v>
+      </c>
+      <c r="H26" s="27"/>
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="35"/>
       <c r="B27" s="24">
         <v>25</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>251</v>
+        <v>90</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>150</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H27" s="11"/>
     </row>
@@ -2442,211 +2479,211 @@
         <v>26</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>97</v>
+        <v>229</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28" s="17" t="s">
         <v>150</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H28" s="11"/>
     </row>
-    <row r="29" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="35"/>
       <c r="B29" s="24">
         <v>27</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>258</v>
+        <v>96</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="H29" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="35"/>
       <c r="B30" s="24">
         <v>28</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="23"/>
+      <c r="C30" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>97</v>
+      </c>
       <c r="E30" s="22" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="17"/>
-      <c r="H30" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>150</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="35"/>
       <c r="B31" s="24">
         <v>29</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>101</v>
+        <v>257</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>58</v>
+        <v>111</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="35"/>
       <c r="B32" s="24">
-        <v>31</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D32" s="23" t="s">
-        <v>137</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>149</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="35"/>
       <c r="B33" s="24">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="26" t="s">
-        <v>149</v>
+        <v>58</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="35"/>
       <c r="B34" s="24">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>103</v>
+        <v>139</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>223</v>
+        <v>137</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>153</v>
+        <v>115</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="76.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="35"/>
       <c r="B35" s="24">
-        <v>34</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>263</v>
+        <v>33</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>140</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>228</v>
+        <v>116</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>149</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>136</v>
+      </c>
+      <c r="H35" s="27"/>
+    </row>
+    <row r="36" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="35"/>
       <c r="B36" s="24">
-        <v>35</v>
-      </c>
-      <c r="C36" s="22" t="s">
-        <v>252</v>
+        <v>34</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>103</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>265</v>
+        <v>223</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="10" t="s">
-        <v>267</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="35"/>
       <c r="B37" s="24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>128</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>150</v>
@@ -2659,7 +2696,7 @@
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="35"/>
       <c r="B38" s="24">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>105</v>
@@ -2681,31 +2718,33 @@
     <row r="39" spans="1:8" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="35"/>
       <c r="B39" s="24">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="22" t="s">
+        <v>277</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>232</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>233</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>65</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H39" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="35"/>
       <c r="B40" s="24">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>66</v>
@@ -2721,7 +2760,7 @@
     <row r="41" spans="1:8" ht="80.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="35"/>
       <c r="B41" s="24">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>155</v>
@@ -2733,19 +2772,19 @@
         <v>110</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>224</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="35"/>
       <c r="B42" s="24">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>42</v>
@@ -2765,13 +2804,13 @@
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="35"/>
       <c r="B43" s="24">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>161</v>
       </c>
       <c r="D43" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>142</v>
@@ -2785,13 +2824,13 @@
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="35"/>
       <c r="B44" s="24">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>162</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>143</v>
@@ -2805,7 +2844,7 @@
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="35"/>
       <c r="B45" s="24">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>132</v>
@@ -2827,13 +2866,13 @@
     <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="35"/>
       <c r="B46" s="24">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>133</v>
       </c>
       <c r="D46" s="22" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>68</v>
@@ -2849,13 +2888,13 @@
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="35"/>
       <c r="B47" s="24">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>167</v>
@@ -2869,7 +2908,7 @@
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="35"/>
       <c r="B48" s="24">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>144</v>
@@ -2887,7 +2926,7 @@
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="35"/>
       <c r="B49" s="24">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>145</v>
@@ -2905,7 +2944,7 @@
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="35"/>
       <c r="B50" s="24">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>231</v>
@@ -2923,73 +2962,91 @@
     <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.15">
       <c r="A51" s="32"/>
       <c r="B51" s="24">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C51" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="D51" s="23" t="s">
         <v>241</v>
-      </c>
-      <c r="D51" s="23" t="s">
-        <v>242</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="17" t="s">
         <v>171</v>
       </c>
       <c r="G51" s="26"/>
-      <c r="H51" s="27"/>
-    </row>
-    <row r="52" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="33" t="s">
+      <c r="H51" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="32"/>
+      <c r="B52" s="24">
+        <v>50</v>
+      </c>
+      <c r="C52" s="23"/>
+      <c r="D52" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="E52" s="22"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="H52" s="27"/>
+    </row>
+    <row r="53" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="25">
+      <c r="B53" s="25">
         <v>1</v>
       </c>
-      <c r="C52" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="D52" s="23" t="s">
+      <c r="C53" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="D53" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E53" s="23" t="s">
         <v>69</v>
-      </c>
-      <c r="F52" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="G52" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="H52" s="27"/>
-    </row>
-    <row r="53" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="33"/>
-      <c r="B53" s="25">
-        <v>2</v>
-      </c>
-      <c r="C53" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>243</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>70</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>153</v>
       </c>
       <c r="G53" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="H53" s="27"/>
+    </row>
+    <row r="54" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="33"/>
+      <c r="B54" s="25">
+        <v>2</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="H53" s="27"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="D58"/>
+      <c r="H54" s="27"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D59"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A53:A54"/>
     <mergeCell ref="A2:A50"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3020,45 +3077,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="39" t="s">
         <v>176</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C1" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="40" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="41"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="40"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="39" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="41"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="7" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="41"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="6" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="39" t="s">
         <v>175</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -3066,28 +3123,28 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="41"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="6" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="39" t="s">
         <v>174</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="40" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="41"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
@@ -3098,315 +3155,315 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="36" t="s">
         <v>172</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="40" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="42"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="36" t="s">
         <v>181</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="40" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="42"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="40"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="37" t="s">
         <v>178</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="40" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="44"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="44"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="41" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="42"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="42"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="42"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C19" s="38"/>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="42"/>
+      <c r="A20" s="36"/>
       <c r="B20" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C20" s="38"/>
+      <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="42"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C21" s="38"/>
+      <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="42"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="C22" s="38"/>
+      <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="42"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C23" s="38"/>
+      <c r="C23" s="42"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="42"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="42"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="36" t="s">
         <v>194</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="38"/>
+      <c r="C25" s="42"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="42"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="38"/>
+      <c r="C26" s="42"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="42"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C27" s="38"/>
+      <c r="C27" s="42"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="42"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="38"/>
+      <c r="C28" s="42"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="42"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="38"/>
+      <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="42"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="38"/>
+      <c r="C30" s="42"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="42"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C31" s="38"/>
+      <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="42"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C32" s="38"/>
+      <c r="C32" s="42"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="C33" s="38"/>
+      <c r="C33" s="42"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="42"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="38"/>
+      <c r="C34" s="42"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="42"/>
+      <c r="A35" s="36"/>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="38"/>
+      <c r="C35" s="42"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="42"/>
+      <c r="A36" s="36"/>
       <c r="B36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="38"/>
+      <c r="C36" s="42"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="42"/>
+      <c r="A37" s="36"/>
       <c r="B37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="38"/>
+      <c r="C37" s="42"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="42"/>
+      <c r="A38" s="36"/>
       <c r="B38" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="38"/>
+      <c r="C38" s="42"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="42"/>
+      <c r="A39" s="36"/>
       <c r="B39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="38"/>
+      <c r="C39" s="42"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="42"/>
+      <c r="A40" s="36"/>
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="38"/>
+      <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="38"/>
+      <c r="C41" s="42"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="42"/>
+      <c r="A42" s="36"/>
       <c r="B42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="38"/>
+      <c r="C42" s="42"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="42"/>
+      <c r="A43" s="36"/>
       <c r="B43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="38"/>
+      <c r="C43" s="42"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="42"/>
+      <c r="A44" s="36"/>
       <c r="B44" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="38"/>
+      <c r="C44" s="42"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="42"/>
+      <c r="A45" s="36"/>
       <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="38"/>
+      <c r="C45" s="42"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="42"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="38"/>
+      <c r="C46" s="42"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="42"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="38"/>
+      <c r="C47" s="42"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="42"/>
+      <c r="A48" s="36"/>
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="39"/>
+      <c r="C48" s="43"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C17:C48"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="A25:A32"/>
     <mergeCell ref="A33:A40"/>
     <mergeCell ref="A41:A48"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A24"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C17:C48"/>
-    <mergeCell ref="C15:C16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update the command list for 2.1.11 and 2.1.12 seperately
</commit_message>
<xml_diff>
--- a/R1_test_command_list_V2.0_for_2.1.11.xlsx
+++ b/R1_test_command_list_V2.0_for_2.1.11.xlsx
@@ -156,22 +156,10 @@
     </r>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/button_f_check.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/set_shutdown.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>set_battery_poweron.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Play DUT memory audio file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>set_shipping_mode.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -273,14 +261,6 @@
   </si>
   <si>
     <t>adb shell /etc/factory-test/r1/get_wlan0_mac.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/connect_wifi.sh office_wifi 1234</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/set_wlan0_mac.sh b0:67:2f:29:2c:ac</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -983,10 +963,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_charger_off.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/set_bt0_mac.sh b0:67:2f:29:2c:af</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1008,10 +984,6 @@
   </si>
   <si>
     <t>adb shell /etc/factory-test/r1/set_standby_mode.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/get_bt_name.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1050,10 +1022,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/get_sw_version.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>reboot.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1087,14 +1055,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_bt_volume.sh  &lt;volume&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/get_bt_volume.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/get_bat_sn.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1103,18 +1063,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Set DUT enter loop back mode and DUT play audio and record by itself</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Set the microphone mute</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/set_mic_mute.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/set_shipping_mode.sh</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1151,18 +1103,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/record_play.sh  &lt;recording time&gt; &lt;song.wav&gt;  &lt;volume value&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve">Changed in 2.1.11, please add a volume value parameter (from -120 - 0, min - max) in the end of this command,  and to set the volume value </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>added in 2.1.11, this command is for looping back mode. The volume value parameter range (from -120 - 0, min - max)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Currently green LED in the end of the test is an indication of a success. Later we maye have more data to share after burn in test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1172,16 +1116,6 @@
   </si>
   <si>
     <t>CONNECT_b</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added in 2.1.11 version for set BT volume only. 
-The volume range changes to (-120 - 0), not (0 - 1.0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added in 2.1.11 version for get BT volume only.
-The volume range changes to (-120 - 0), not (0 - 1.0)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1207,6 +1141,74 @@
   </si>
   <si>
     <t>set_standby_mode.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Play DUT memory audio file</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/button_f_c+D13+D2:D+D2:D44</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/connect_wifi.sh office_wifi 1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_sw_version.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_shutdown.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_wlan0_mac.sh b0:67:2f:29:2c:ac</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_bt_volume.sh  &lt;volume value&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_charger_off.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/set_mic_mute.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_bt_name.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added in 2.1.11, this command is for looping back mode. The volume value parameter range (from -120 - 0, min - max)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added in 2.1.11 version for set BT volume only. 
+The volume value range changed to (-120 - 0), not (0 - 1.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added in 2.1.11 version for get BT volume only.
+The volume value range changed to (-120 - 0), not (0 - 1.0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/get_bt_volume.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. adb shell /etc/factory-test/r1/mic_record_init.sh
+2. adb shell /etc/factory-test/r1/mic_record_start.sh &lt;recording time&gt; 
+&amp; adb shell /etc/factory-test/r1/play_file.sh  &lt;song.wav&gt;  &lt;volume value&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Set DUT enter loop back mode and DUT play audio and record by itself+E21:H21E21:K21E21:J21E21:I21E21:H21</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1214,7 +1216,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1305,16 +1307,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1355,11 +1349,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1444,13 +1433,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1572,12 +1558,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1882,8 +1864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1891,8 +1873,7 @@
     <col min="1" max="1" width="6.875" style="13" customWidth="1"/>
     <col min="2" max="2" width="6" style="21" customWidth="1"/>
     <col min="3" max="3" width="37" style="13" customWidth="1"/>
-    <col min="4" max="4" width="46.625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="46.25" style="13" customWidth="1"/>
+    <col min="4" max="5" width="75.75" style="13" customWidth="1"/>
     <col min="6" max="6" width="30.875" style="13" customWidth="1"/>
     <col min="7" max="7" width="60.375" style="13" customWidth="1"/>
     <col min="8" max="8" width="44.625" style="12" customWidth="1"/>
@@ -1901,7 +1882,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>15</v>
@@ -1916,33 +1897,33 @@
         <v>14</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="24">
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>37</v>
+        <v>263</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G2" s="17"/>
       <c r="H2" s="27"/>
@@ -1953,19 +1934,19 @@
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>74</v>
+        <v>102</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H3" s="27"/>
     </row>
@@ -1977,17 +1958,17 @@
       <c r="C4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>268</v>
+      <c r="D4" s="16" t="s">
+        <v>254</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="H4" s="27"/>
     </row>
@@ -1999,17 +1980,17 @@
       <c r="C5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>244</v>
+      <c r="D5" s="16" t="s">
+        <v>236</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H5" s="27"/>
     </row>
@@ -2019,23 +2000,23 @@
         <v>5</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="35"/>
       <c r="B7" s="24">
         <v>6</v>
@@ -2043,14 +2024,14 @@
       <c r="C7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>239</v>
+      <c r="D7" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="27"/>
@@ -2059,14 +2040,14 @@
       <c r="A8" s="35"/>
       <c r="B8" s="24"/>
       <c r="C8" s="19"/>
-      <c r="D8" s="17" t="s">
-        <v>160</v>
+      <c r="D8" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="27"/>
@@ -2077,19 +2058,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="17" t="s">
         <v>73</v>
       </c>
+      <c r="D9" s="16" t="s">
+        <v>70</v>
+      </c>
       <c r="E9" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H9" s="27"/>
     </row>
@@ -2101,17 +2082,17 @@
       <c r="C10" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="17" t="s">
-        <v>245</v>
+      <c r="D10" s="16" t="s">
+        <v>237</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H10" s="27"/>
     </row>
@@ -2121,19 +2102,19 @@
         <v>9</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>246</v>
+        <v>76</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>238</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H11" s="27"/>
     </row>
@@ -2143,19 +2124,19 @@
         <v>10</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>227</v>
+        <v>77</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>221</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H12" s="27"/>
     </row>
@@ -2165,16 +2146,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>217</v>
+        <v>119</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>212</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="27"/>
@@ -2185,16 +2166,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>243</v>
+        <v>141</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>235</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="27"/>
@@ -2205,16 +2186,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>219</v>
+        <v>183</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="27"/>
@@ -2227,17 +2208,17 @@
       <c r="C16" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>38</v>
+      <c r="D16" s="16" t="s">
+        <v>266</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H16" s="27"/>
     </row>
@@ -2247,17 +2228,17 @@
         <v>15</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>75</v>
+        <v>213</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>267</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H17" s="11"/>
     </row>
@@ -2267,18 +2248,18 @@
         <v>16</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>235</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>248</v>
+        <v>228</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>268</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="F18" s="31"/>
       <c r="G18" s="17"/>
       <c r="H18" s="10" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -2287,18 +2268,18 @@
         <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>249</v>
+        <v>230</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>275</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="17"/>
       <c r="H19" s="10" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.15">
@@ -2307,22 +2288,22 @@
         <v>18</v>
       </c>
       <c r="C20" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="E20" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>40</v>
-      </c>
       <c r="F20" s="22" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -2331,18 +2312,18 @@
         <v>19</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>264</v>
+        <v>241</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>276</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>252</v>
+        <v>277</v>
       </c>
       <c r="F21" s="21"/>
       <c r="G21" s="17"/>
       <c r="H21" s="10" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2351,17 +2332,17 @@
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>220</v>
+        <v>81</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>215</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H22" s="27"/>
     </row>
@@ -2371,17 +2352,17 @@
         <v>21</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>125</v>
+        <v>82</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="E23" s="22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="H23" s="27"/>
     </row>
@@ -2391,19 +2372,19 @@
         <v>22</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>225</v>
+        <v>121</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>220</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H24" s="27"/>
     </row>
@@ -2413,19 +2394,19 @@
         <v>23</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="23" t="s">
-        <v>156</v>
+        <v>83</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>151</v>
       </c>
       <c r="E25" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="G25" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="H25" s="27"/>
     </row>
@@ -2435,19 +2416,19 @@
         <v>24</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>221</v>
+        <v>84</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>216</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H26" s="27"/>
     </row>
@@ -2457,19 +2438,19 @@
         <v>25</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>90</v>
+        <v>87</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="E27" s="22" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H27" s="11"/>
     </row>
@@ -2479,19 +2460,19 @@
         <v>26</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>229</v>
+        <v>89</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>223</v>
       </c>
       <c r="E28" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H28" s="11"/>
     </row>
@@ -2501,19 +2482,19 @@
         <v>27</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="23" t="s">
-        <v>250</v>
+        <v>91</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>240</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H29" s="11"/>
     </row>
@@ -2523,19 +2504,19 @@
         <v>28</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="23" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>92</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="H30" s="11"/>
     </row>
@@ -2545,22 +2526,22 @@
         <v>29</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>230</v>
+        <v>245</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>224</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2569,18 +2550,18 @@
         <v>30</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="23"/>
+        <v>37</v>
+      </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -2589,19 +2570,19 @@
         <v>31</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>222</v>
+        <v>96</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>217</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H33" s="27"/>
     </row>
@@ -2611,19 +2592,19 @@
         <v>32</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>132</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H34" s="27"/>
     </row>
@@ -2633,19 +2614,19 @@
         <v>33</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>226</v>
+        <v>135</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>269</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H35" s="27"/>
     </row>
@@ -2655,19 +2636,19 @@
         <v>34</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>223</v>
+        <v>98</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H36" s="27"/>
     </row>
@@ -2677,19 +2658,19 @@
         <v>35</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>254</v>
+        <v>123</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>270</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G37" s="26" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H37" s="27"/>
     </row>
@@ -2699,19 +2680,19 @@
         <v>36</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>135</v>
+        <v>100</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>130</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F38" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G38" s="26" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H38" s="27"/>
     </row>
@@ -2721,39 +2702,39 @@
         <v>37</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>232</v>
+        <v>261</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>226</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="17"/>
       <c r="H39" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40" s="35"/>
       <c r="B40" s="24">
         <v>38</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>255</v>
+        <v>38</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>243</v>
       </c>
       <c r="E40" s="22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H40" s="11"/>
     </row>
@@ -2763,22 +2744,22 @@
         <v>39</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>134</v>
+        <v>150</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="E41" s="22" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
@@ -2787,18 +2768,18 @@
         <v>40</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="22"/>
+        <v>39</v>
+      </c>
+      <c r="D42" s="16"/>
       <c r="E42" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F42" s="29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G42" s="17"/>
       <c r="H42" s="10" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2807,16 +2788,16 @@
         <v>41</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="D43" s="22" t="s">
-        <v>258</v>
+        <v>156</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>246</v>
       </c>
       <c r="E43" s="22" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F43" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G43" s="17"/>
       <c r="H43" s="27"/>
@@ -2827,80 +2808,80 @@
         <v>42</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="D44" s="22" t="s">
-        <v>259</v>
+        <v>157</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>247</v>
       </c>
       <c r="E44" s="22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F44" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G44" s="17"/>
       <c r="H44" s="27"/>
     </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A45" s="35"/>
       <c r="B45" s="24">
         <v>43</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="22" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="D45" s="16" t="s">
+        <v>124</v>
       </c>
       <c r="E45" s="22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G45" s="26" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H45" s="27"/>
     </row>
-    <row r="46" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A46" s="35"/>
       <c r="B46" s="24">
         <v>44</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D46" s="22" t="s">
-        <v>260</v>
+        <v>128</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="E46" s="22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F46" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="G46" s="26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H46" s="27"/>
     </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47" s="35"/>
       <c r="B47" s="24">
         <v>45</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>233</v>
+        <v>249</v>
+      </c>
+      <c r="D47" s="16" t="s">
+        <v>271</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F47" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G47" s="26"/>
       <c r="H47" s="27"/>
@@ -2911,14 +2892,14 @@
         <v>46</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D48" s="23"/>
+        <v>139</v>
+      </c>
+      <c r="D48" s="16"/>
       <c r="E48" s="22" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F48" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G48" s="26"/>
       <c r="H48" s="27"/>
@@ -2929,14 +2910,14 @@
         <v>47</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="D49" s="23"/>
+        <v>140</v>
+      </c>
+      <c r="D49" s="16"/>
       <c r="E49" s="22" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G49" s="26"/>
       <c r="H49" s="27"/>
@@ -2947,36 +2928,36 @@
         <v>48</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="D50" s="23"/>
+        <v>225</v>
+      </c>
+      <c r="D50" s="16"/>
       <c r="E50" s="22" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G50" s="26"/>
       <c r="H50" s="27"/>
     </row>
-    <row r="51" spans="1:8" ht="21" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" ht="27" x14ac:dyDescent="0.15">
       <c r="A51" s="32"/>
       <c r="B51" s="24">
         <v>49</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="D51" s="23" t="s">
-        <v>241</v>
+        <v>232</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>233</v>
       </c>
       <c r="E51" s="22"/>
       <c r="F51" s="17" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G51" s="26"/>
       <c r="H51" s="10" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2985,37 +2966,37 @@
         <v>50</v>
       </c>
       <c r="C52" s="23"/>
-      <c r="D52" s="45" t="s">
-        <v>275</v>
+      <c r="D52" s="16" t="s">
+        <v>259</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="17"/>
       <c r="G52" s="26" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="H52" s="27"/>
     </row>
     <row r="53" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B53" s="25">
         <v>1</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>272</v>
-      </c>
-      <c r="D53" s="23" t="s">
-        <v>108</v>
+        <v>256</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F53" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G53" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H53" s="27"/>
     </row>
@@ -3025,19 +3006,19 @@
         <v>2</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="23" t="s">
-        <v>242</v>
+        <v>104</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>234</v>
       </c>
       <c r="E54" s="23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F54" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H54" s="27"/>
     </row>
@@ -3078,19 +3059,19 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="39" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="39"/>
       <c r="B2" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C2" s="40"/>
     </row>
@@ -3099,112 +3080,112 @@
         <v>33</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="39"/>
       <c r="B4" s="7" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="39"/>
       <c r="B5" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="39" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="39"/>
       <c r="B7" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="39" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C8" s="40" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="39"/>
       <c r="B9" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C9" s="40"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="36" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="36"/>
       <c r="B12" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C12" s="40"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="36" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C13" s="40" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="36"/>
       <c r="B14" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C14" s="40"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="37" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="38"/>
       <c r="B16" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C16" s="44"/>
     </row>
@@ -3213,7 +3194,7 @@
         <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C17" s="41" t="s">
         <v>36</v>
@@ -3222,42 +3203,42 @@
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="36"/>
       <c r="B18" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C18" s="42"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="36"/>
       <c r="B19" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="36"/>
       <c r="B20" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C20" s="42"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="36"/>
       <c r="B21" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C21" s="42"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="36"/>
       <c r="B22" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C22" s="42"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="36"/>
       <c r="B23" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C23" s="42"/>
     </row>
@@ -3270,59 +3251,59 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="36" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C25" s="42"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="36"/>
       <c r="B26" s="6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C26" s="42"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="36"/>
       <c r="B27" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C27" s="42"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="36"/>
       <c r="B28" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C28" s="42"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="36"/>
       <c r="B29" s="6" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="36"/>
       <c r="B30" s="6" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C30" s="42"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="36"/>
       <c r="B31" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="36"/>
       <c r="B32" s="6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C32" s="42"/>
     </row>
@@ -3331,7 +3312,7 @@
         <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C33" s="42"/>
     </row>

</xml_diff>

<commit_message>
Update command list for 2.1.11 and 2.1.12 record play function
</commit_message>
<xml_diff>
--- a/R1_test_command_list_V2.0_for_2.1.11.xlsx
+++ b/R1_test_command_list_V2.0_for_2.1.11.xlsx
@@ -1047,10 +1047,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/mic_record_init.sh                                adb shell /etc/factory-test/r1/mic_record_start.sh 1314</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ACTION_g</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1096,10 +1092,6 @@
   </si>
   <si>
     <t>play_file.sh</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adb shell /etc/factory-test/r1/play_file.sh &lt;song.wav&gt;  &lt;volume value&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1148,10 +1140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>adb shell /etc/factory-test/r1/button_f_c+D13+D2:D+D2:D44</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>adb shell /etc/factory-test/r1/connect_wifi.sh office_wifi 1234</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1202,13 +1190,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>adb shell /etc/factory-test/r1/play_file.sh &lt;song.wav&gt;  &lt;volume value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/mic_record_init.sh                                adb shell /etc/factory-test/r1/mic_record_start.sh 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adb shell /etc/factory-test/r1/button_f_check.sh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1. adb shell /etc/factory-test/r1/mic_record_init.sh
-2. adb shell /etc/factory-test/r1/mic_record_start.sh &lt;recording time&gt; 
-&amp; adb shell /etc/factory-test/r1/play_file.sh  &lt;song.wav&gt;  &lt;volume value&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Set DUT enter loop back mode and DUT play audio and record by itself+E21:H21E21:K21E21:J21E21:I21E21:H21</t>
+2. adb shell busybox nohup /etc/factory-test/r1/mic_record_start.sh  &lt;recording time&gt;
+3. adb shell /etc/factory-test/r1/play_file.sh  &lt;song.wav&gt;  &lt;volume value&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Set DUT enter loop back mode and DUT play audio and record by itself. 
+Please running the step 3 immeidately after step 2.
+Example:
+adb shell /etc/factory-test/r1/mic_record_init.sh
+adb shell  busybox nohup /etc/factory-test/r1/mic_record_start.sh  20
+adb shell "/etc/factory-test/r1/play_file.sh  /data/ota-file/Chains.wav  0 
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1531,6 +1537,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1539,24 +1563,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1864,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:G21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1917,7 +1923,7 @@
         <v>68</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>9</v>
@@ -1937,7 +1943,7 @@
         <v>102</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E3" s="17" t="s">
         <v>161</v>
@@ -1959,7 +1965,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E4" s="17" t="s">
         <v>41</v>
@@ -2025,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>11</v>
@@ -2105,7 +2111,7 @@
         <v>76</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="E11" s="16" t="s">
         <v>10</v>
@@ -2209,7 +2215,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>5</v>
@@ -2231,7 +2237,7 @@
         <v>213</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E17" s="16" t="s">
         <v>8</v>
@@ -2251,7 +2257,7 @@
         <v>228</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>229</v>
@@ -2259,7 +2265,7 @@
       <c r="F18" s="31"/>
       <c r="G18" s="17"/>
       <c r="H18" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="54" x14ac:dyDescent="0.15">
@@ -2271,7 +2277,7 @@
         <v>230</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E19" s="16" t="s">
         <v>231</v>
@@ -2279,7 +2285,7 @@
       <c r="F19" s="31"/>
       <c r="G19" s="17"/>
       <c r="H19" s="10" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.15">
@@ -2288,13 +2294,13 @@
         <v>18</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F20" s="22" t="s">
         <v>222</v>
@@ -2303,16 +2309,16 @@
         <v>227</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="84" x14ac:dyDescent="0.15">
       <c r="A21" s="35"/>
       <c r="B21" s="24">
         <v>19</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>276</v>
@@ -2323,10 +2329,10 @@
       <c r="F21" s="21"/>
       <c r="G21" s="17"/>
       <c r="H21" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="35"/>
       <c r="B22" s="24">
         <v>20</v>
@@ -2346,7 +2352,7 @@
       </c>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="35"/>
       <c r="B23" s="24">
         <v>21</v>
@@ -2485,7 +2491,7 @@
         <v>91</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E29" s="22" t="s">
         <v>53</v>
@@ -2526,7 +2532,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>224</v>
@@ -2617,7 +2623,7 @@
         <v>135</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E35" s="22" t="s">
         <v>111</v>
@@ -2661,10 +2667,10 @@
         <v>123</v>
       </c>
       <c r="D37" s="16" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>145</v>
@@ -2702,7 +2708,7 @@
         <v>37</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D39" s="16" t="s">
         <v>226</v>
@@ -2713,7 +2719,7 @@
       <c r="F39" s="22"/>
       <c r="G39" s="17"/>
       <c r="H39" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.15">
@@ -2725,7 +2731,7 @@
         <v>38</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>63</v>
@@ -2753,13 +2759,13 @@
         <v>105</v>
       </c>
       <c r="F41" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>219</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.15">
@@ -2791,7 +2797,7 @@
         <v>156</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>137</v>
@@ -2811,7 +2817,7 @@
         <v>157</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>138</v>
@@ -2853,7 +2859,7 @@
         <v>128</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>65</v>
@@ -2872,10 +2878,10 @@
         <v>45</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E47" s="22" t="s">
         <v>162</v>
@@ -2957,7 +2963,7 @@
       </c>
       <c r="G51" s="26"/>
       <c r="H51" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -2967,12 +2973,12 @@
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="16" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="17"/>
       <c r="G52" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H52" s="27"/>
     </row>
@@ -2984,7 +2990,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D53" s="16" t="s">
         <v>103</v>
@@ -3058,45 +3064,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>171</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="C1" s="40" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="39"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="36"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="39"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="7" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="39"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="6" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="41" t="s">
         <v>170</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -3104,28 +3110,28 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="39"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="6" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>169</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="36" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C9" s="40"/>
+      <c r="C9" s="36"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="30" t="s">
@@ -3136,315 +3142,315 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="42" t="s">
         <v>167</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="36" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="36"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C12" s="40"/>
+      <c r="C12" s="36"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="42" t="s">
         <v>176</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="36" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="36"/>
+      <c r="A14" s="42"/>
       <c r="B14" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="36"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="43" t="s">
         <v>173</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="36" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="38"/>
+      <c r="A16" s="44"/>
       <c r="B16" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="40"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="42" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="37" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="36"/>
+      <c r="A18" s="42"/>
       <c r="B18" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C18" s="42"/>
+      <c r="C18" s="38"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="36"/>
+      <c r="A19" s="42"/>
       <c r="B19" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="38"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="36"/>
+      <c r="A20" s="42"/>
       <c r="B20" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C20" s="42"/>
+      <c r="C20" s="38"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="36"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="38"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="36"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="38"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="36"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="38"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="36"/>
+      <c r="A24" s="42"/>
       <c r="B24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="38"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="42" t="s">
         <v>189</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="42"/>
+      <c r="C25" s="38"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="36"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C26" s="42"/>
+      <c r="C26" s="38"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="36"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="38"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="36"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="C28" s="42"/>
+      <c r="C28" s="38"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="36"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="38"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="36"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="38"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="36"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C31" s="42"/>
+      <c r="C31" s="38"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="36"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="38"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="42" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="42"/>
+      <c r="C33" s="38"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="36"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="42"/>
+      <c r="C34" s="38"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="36"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="42"/>
+      <c r="C35" s="38"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="36"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="38"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="36"/>
+      <c r="A37" s="42"/>
       <c r="B37" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="38"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="36"/>
+      <c r="A38" s="42"/>
       <c r="B38" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="38"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="36"/>
+      <c r="A39" s="42"/>
       <c r="B39" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="42"/>
+      <c r="C39" s="38"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="36"/>
+      <c r="A40" s="42"/>
       <c r="B40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="38"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="42" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="38"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="36"/>
+      <c r="A42" s="42"/>
       <c r="B42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="42"/>
+      <c r="C42" s="38"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="36"/>
+      <c r="A43" s="42"/>
       <c r="B43" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="42"/>
+      <c r="C43" s="38"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="36"/>
+      <c r="A44" s="42"/>
       <c r="B44" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="42"/>
+      <c r="C44" s="38"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="36"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="42"/>
+      <c r="C45" s="38"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A46" s="36"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="42"/>
+      <c r="C46" s="38"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="36"/>
+      <c r="A47" s="42"/>
       <c r="B47" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="42"/>
+      <c r="C47" s="38"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48" s="36"/>
+      <c r="A48" s="42"/>
       <c r="B48" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="43"/>
+      <c r="C48" s="39"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A25:A32"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A41:A48"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A17:A24"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A6:A7"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="C17:C48"/>
     <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A25:A32"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A41:A48"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A17:A24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>